<commit_message>
if you think it, I made a function for it
</commit_message>
<xml_diff>
--- a/data/demand_nodes.xlsx
+++ b/data/demand_nodes.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mitprod-my.sharepoint.com/personal/alandler_mit_edu/Documents/1.013/simulation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{354DA1A0-91C9-254F-8FBB-16A80111756C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{354DA1A0-91C9-254F-8FBB-16A80111756C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3E292D1-F55D-2B41-9759-019ED376C3FF}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="demand_nodes" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -139,8 +149,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -271,6 +281,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -617,8 +634,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -973,11 +991,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AC21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1085,103 +1103,103 @@
         <v>4</v>
       </c>
       <c r="E2">
-        <v>170</v>
+        <v>22</v>
       </c>
       <c r="F2">
         <f>ROUND($E2*F$10,0)</f>
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <f t="shared" ref="G2:AC9" si="0">ROUND($E2*G$10,0)</f>
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="H2">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="I2">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="J2">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>15</v>
       </c>
       <c r="K2">
         <f t="shared" si="0"/>
-        <v>136</v>
+        <v>18</v>
       </c>
       <c r="L2">
         <f t="shared" si="0"/>
-        <v>170</v>
+        <v>22</v>
       </c>
       <c r="M2">
         <f t="shared" si="0"/>
-        <v>170</v>
+        <v>22</v>
       </c>
       <c r="N2">
         <f t="shared" si="0"/>
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="O2">
         <f t="shared" si="0"/>
-        <v>136</v>
+        <v>18</v>
       </c>
       <c r="P2">
         <f t="shared" si="0"/>
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="Q2">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="R2">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="S2">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="T2">
         <f t="shared" si="0"/>
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="U2">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>15</v>
       </c>
       <c r="V2">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>9</v>
       </c>
       <c r="W2">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="X2">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="Y2">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="Z2">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="AA2">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="AB2">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="AC2">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
@@ -1198,103 +1216,103 @@
         <v>6</v>
       </c>
       <c r="E3">
-        <v>220</v>
+        <v>28</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:U9" si="1">ROUND($E3*F$10,0)</f>
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="G3">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="H3">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="I3">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="J3">
         <f t="shared" si="1"/>
-        <v>154</v>
+        <v>20</v>
       </c>
       <c r="K3">
         <f t="shared" si="1"/>
-        <v>176</v>
+        <v>22</v>
       </c>
       <c r="L3">
         <f t="shared" si="1"/>
-        <v>220</v>
+        <v>28</v>
       </c>
       <c r="M3">
         <f t="shared" si="1"/>
-        <v>220</v>
+        <v>28</v>
       </c>
       <c r="N3">
         <f t="shared" si="1"/>
-        <v>198</v>
+        <v>25</v>
       </c>
       <c r="O3">
         <f t="shared" si="1"/>
-        <v>176</v>
+        <v>22</v>
       </c>
       <c r="P3">
         <f t="shared" si="1"/>
-        <v>132</v>
+        <v>17</v>
       </c>
       <c r="Q3">
         <f t="shared" si="1"/>
-        <v>110</v>
+        <v>14</v>
       </c>
       <c r="R3">
         <f t="shared" si="1"/>
-        <v>110</v>
+        <v>14</v>
       </c>
       <c r="S3">
         <f t="shared" si="1"/>
-        <v>110</v>
+        <v>14</v>
       </c>
       <c r="T3">
         <f t="shared" si="1"/>
-        <v>132</v>
+        <v>17</v>
       </c>
       <c r="U3">
         <f t="shared" si="1"/>
-        <v>154</v>
+        <v>20</v>
       </c>
       <c r="V3">
         <f t="shared" si="0"/>
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="W3">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="X3">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="Y3">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="Z3">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="AA3">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="AB3">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="AC3">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.2">
@@ -1311,103 +1329,103 @@
         <v>9</v>
       </c>
       <c r="E4">
-        <v>210</v>
+        <v>27</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>147</v>
+        <v>19</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>168</v>
+        <v>22</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
-        <v>210</v>
+        <v>27</v>
       </c>
       <c r="M4">
         <f t="shared" si="0"/>
-        <v>210</v>
+        <v>27</v>
       </c>
       <c r="N4">
         <f t="shared" si="0"/>
-        <v>189</v>
+        <v>24</v>
       </c>
       <c r="O4">
         <f t="shared" si="0"/>
-        <v>168</v>
+        <v>22</v>
       </c>
       <c r="P4">
         <f t="shared" si="0"/>
-        <v>126</v>
+        <v>16</v>
       </c>
       <c r="Q4">
         <f t="shared" si="0"/>
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="R4">
         <f t="shared" si="0"/>
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="S4">
         <f t="shared" si="0"/>
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="T4">
         <f t="shared" si="0"/>
-        <v>126</v>
+        <v>16</v>
       </c>
       <c r="U4">
         <f t="shared" si="0"/>
-        <v>147</v>
+        <v>19</v>
       </c>
       <c r="V4">
         <f t="shared" si="0"/>
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="W4">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="X4">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="Y4">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="Z4">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="AA4">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="AB4">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="AC4">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.2">
@@ -1424,103 +1442,103 @@
         <v>6</v>
       </c>
       <c r="E5">
-        <v>170</v>
+        <v>22</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>15</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>136</v>
+        <v>18</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>170</v>
+        <v>22</v>
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
-        <v>170</v>
+        <v>22</v>
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="O5">
         <f t="shared" si="0"/>
-        <v>136</v>
+        <v>18</v>
       </c>
       <c r="P5">
         <f t="shared" si="0"/>
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="Q5">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="R5">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="S5">
         <f t="shared" si="0"/>
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="T5">
         <f t="shared" si="0"/>
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="U5">
         <f t="shared" si="0"/>
-        <v>119</v>
+        <v>15</v>
       </c>
       <c r="V5">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>9</v>
       </c>
       <c r="W5">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="X5">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="Y5">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="Z5">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="AA5">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="AB5">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="AC5">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
@@ -1537,103 +1555,103 @@
         <v>2</v>
       </c>
       <c r="E6">
-        <v>150</v>
+        <v>19</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G6">
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="O6">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>105</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="0"/>
-        <v>150</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="0"/>
-        <v>135</v>
-      </c>
-      <c r="O6">
-        <f t="shared" si="0"/>
-        <v>120</v>
-      </c>
       <c r="P6">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>11</v>
       </c>
       <c r="Q6">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="R6">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="S6">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="T6">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>11</v>
       </c>
       <c r="U6">
         <f t="shared" si="0"/>
-        <v>105</v>
+        <v>13</v>
       </c>
       <c r="V6">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="W6">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="X6">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="Y6">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="Z6">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="AA6">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="AB6">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="AC6">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
@@ -1650,103 +1668,103 @@
         <v>4</v>
       </c>
       <c r="E7">
-        <v>290</v>
+        <v>37</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>6</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="J7">
         <f t="shared" si="0"/>
-        <v>203</v>
+        <v>26</v>
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>232</v>
+        <v>30</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>290</v>
+        <v>37</v>
       </c>
       <c r="M7">
         <f t="shared" si="0"/>
-        <v>290</v>
+        <v>37</v>
       </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>261</v>
+        <v>33</v>
       </c>
       <c r="O7">
         <f t="shared" si="0"/>
-        <v>232</v>
+        <v>30</v>
       </c>
       <c r="P7">
         <f t="shared" si="0"/>
-        <v>174</v>
+        <v>22</v>
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
-        <v>145</v>
+        <v>19</v>
       </c>
       <c r="R7">
         <f t="shared" si="0"/>
-        <v>145</v>
+        <v>19</v>
       </c>
       <c r="S7">
         <f t="shared" si="0"/>
-        <v>145</v>
+        <v>19</v>
       </c>
       <c r="T7">
         <f t="shared" si="0"/>
-        <v>174</v>
+        <v>22</v>
       </c>
       <c r="U7">
         <f t="shared" si="0"/>
-        <v>203</v>
+        <v>26</v>
       </c>
       <c r="V7">
         <f t="shared" si="0"/>
-        <v>116</v>
+        <v>15</v>
       </c>
       <c r="W7">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="X7">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="Y7">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="Z7">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="AA7">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="AB7">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="AC7">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
@@ -1763,103 +1781,103 @@
         <v>8</v>
       </c>
       <c r="E8">
-        <v>310</v>
+        <v>39</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="G8">
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="O8">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>78</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="0"/>
-        <v>217</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="0"/>
-        <v>248</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="0"/>
-        <v>310</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="0"/>
-        <v>310</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="0"/>
-        <v>279</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="0"/>
-        <v>248</v>
-      </c>
       <c r="P8">
         <f t="shared" si="0"/>
-        <v>186</v>
+        <v>23</v>
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="R8">
         <f t="shared" si="0"/>
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="S8">
         <f t="shared" si="0"/>
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="T8">
         <f t="shared" si="0"/>
-        <v>186</v>
+        <v>23</v>
       </c>
       <c r="U8">
         <f t="shared" si="0"/>
-        <v>217</v>
+        <v>27</v>
       </c>
       <c r="V8">
         <f t="shared" si="0"/>
-        <v>124</v>
+        <v>16</v>
       </c>
       <c r="W8">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="X8">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="Y8">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="Z8">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="AA8">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="AB8">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="AC8">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
@@ -1876,103 +1894,103 @@
         <v>6</v>
       </c>
       <c r="E9">
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G9">
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="O9">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="0"/>
-        <v>140</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="0"/>
-        <v>160</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="0"/>
-        <v>200</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="0"/>
-        <v>180</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="0"/>
-        <v>160</v>
-      </c>
       <c r="P9">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>15</v>
       </c>
       <c r="Q9">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="R9">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="S9">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="T9">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>15</v>
       </c>
       <c r="U9">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>18</v>
       </c>
       <c r="V9">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="W9">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="X9">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="Y9">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="Z9">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="AA9">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="AB9">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="AC9">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
@@ -2055,104 +2073,128 @@
       </c>
       <c r="E11">
         <f>SUM(F11:AC11)</f>
-        <v>17894</v>
+        <v>2294</v>
       </c>
       <c r="F11">
         <f>SUM(F2:F9)</f>
-        <v>172</v>
+        <v>23</v>
       </c>
       <c r="G11">
         <f t="shared" ref="G11:AC11" si="2">SUM(G2:G9)</f>
-        <v>172</v>
+        <v>23</v>
       </c>
       <c r="H11">
         <f t="shared" si="2"/>
-        <v>261</v>
+        <v>33</v>
       </c>
       <c r="I11">
         <f t="shared" si="2"/>
-        <v>433</v>
+        <v>56</v>
       </c>
       <c r="J11">
         <f t="shared" si="2"/>
-        <v>1204</v>
+        <v>153</v>
       </c>
       <c r="K11">
         <f t="shared" si="2"/>
-        <v>1376</v>
+        <v>176</v>
       </c>
       <c r="L11">
         <f t="shared" si="2"/>
-        <v>1720</v>
+        <v>219</v>
       </c>
       <c r="M11">
         <f t="shared" si="2"/>
-        <v>1720</v>
+        <v>219</v>
       </c>
       <c r="N11">
         <f t="shared" si="2"/>
-        <v>1548</v>
+        <v>197</v>
       </c>
       <c r="O11">
         <f t="shared" si="2"/>
-        <v>1376</v>
+        <v>176</v>
       </c>
       <c r="P11">
         <f t="shared" si="2"/>
-        <v>1032</v>
+        <v>130</v>
       </c>
       <c r="Q11">
         <f t="shared" si="2"/>
-        <v>860</v>
+        <v>112</v>
       </c>
       <c r="R11">
         <f t="shared" si="2"/>
-        <v>860</v>
+        <v>112</v>
       </c>
       <c r="S11">
         <f t="shared" si="2"/>
-        <v>860</v>
+        <v>112</v>
       </c>
       <c r="T11">
         <f t="shared" si="2"/>
-        <v>1032</v>
+        <v>130</v>
       </c>
       <c r="U11">
         <f t="shared" si="2"/>
-        <v>1204</v>
+        <v>153</v>
       </c>
       <c r="V11">
         <f t="shared" si="2"/>
-        <v>688</v>
+        <v>89</v>
       </c>
       <c r="W11">
         <f t="shared" si="2"/>
-        <v>344</v>
+        <v>43</v>
       </c>
       <c r="X11">
         <f t="shared" si="2"/>
-        <v>172</v>
+        <v>23</v>
       </c>
       <c r="Y11">
         <f t="shared" si="2"/>
-        <v>172</v>
+        <v>23</v>
       </c>
       <c r="Z11">
         <f t="shared" si="2"/>
-        <v>172</v>
+        <v>23</v>
       </c>
       <c r="AA11">
         <f t="shared" si="2"/>
-        <v>172</v>
+        <v>23</v>
       </c>
       <c r="AB11">
         <f t="shared" si="2"/>
-        <v>172</v>
+        <v>23</v>
       </c>
       <c r="AC11">
         <f t="shared" si="2"/>
-        <v>172</v>
-      </c>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>